<commit_message>
add other type of transportation
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyemin/Development/CS6795-project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamet\Dropbox (GaTech)\Summer 2018\CS 6795\Project2\CS6795-project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{263457E5-78A4-479B-998D-ABC35A3BAC64}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="18520" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="458" windowWidth="28800" windowHeight="18518" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -84,12 +85,72 @@
   </si>
   <si>
     <t>walk_safety</t>
+  </si>
+  <si>
+    <t>bus_price</t>
+  </si>
+  <si>
+    <t>bus_comfort_level</t>
+  </si>
+  <si>
+    <t>bus_availability</t>
+  </si>
+  <si>
+    <t>bus_accessability</t>
+  </si>
+  <si>
+    <t>bus_safety</t>
+  </si>
+  <si>
+    <t>uber_price</t>
+  </si>
+  <si>
+    <t>uber_comfort_level</t>
+  </si>
+  <si>
+    <t>uber_availability</t>
+  </si>
+  <si>
+    <t>uber_accessability</t>
+  </si>
+  <si>
+    <t>uber_safety</t>
+  </si>
+  <si>
+    <t>train_price</t>
+  </si>
+  <si>
+    <t>train_comfort_level</t>
+  </si>
+  <si>
+    <t>train_availability</t>
+  </si>
+  <si>
+    <t>train_accessability</t>
+  </si>
+  <si>
+    <t>train_safety</t>
+  </si>
+  <si>
+    <t>bike_price</t>
+  </si>
+  <si>
+    <t>bike_comfort_level</t>
+  </si>
+  <si>
+    <t>bike_availability</t>
+  </si>
+  <si>
+    <t>bike_accessability</t>
+  </si>
+  <si>
+    <t>bike_safety</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -141,6 +202,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -408,16 +472,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,28 +539,68 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -554,8 +658,68 @@
       <c r="S2">
         <v>2</v>
       </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>2</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -613,8 +777,68 @@
       <c r="S3">
         <v>0</v>
       </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>2</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -672,8 +896,68 @@
       <c r="S4">
         <v>1</v>
       </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -731,8 +1015,68 @@
       <c r="S5">
         <v>1</v>
       </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>2</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>2</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -790,8 +1134,68 @@
       <c r="S6">
         <v>2</v>
       </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <v>2</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>2</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -849,8 +1253,68 @@
       <c r="S7">
         <v>2</v>
       </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>2</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>2</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>2</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AM7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -908,8 +1372,68 @@
       <c r="S8">
         <v>0</v>
       </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>2</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -967,8 +1491,68 @@
       <c r="S9">
         <v>0</v>
       </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>2</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>2</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1024,6 +1608,66 @@
         <v>1</v>
       </c>
       <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>2</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
         <v>0</v>
       </c>
     </row>

</xml_diff>